<commit_message>
Ajustado coluna de classificação de risco
</commit_message>
<xml_diff>
--- a/resumo_clusters_com_perfil_emprestimo_e_condicao_pagador.xlsx
+++ b/resumo_clusters_com_perfil_emprestimo_e_condicao_pagador.xlsx
@@ -616,12 +616,12 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Bom Pagador</t>
+          <t>Médio Pagador</t>
         </is>
       </c>
     </row>
@@ -691,12 +691,12 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Muito Alto</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Médio Pagador</t>
+          <t>Mal Pagador</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Bom Pagador</t>
+          <t>Médio Pagador</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Bom Pagador</t>
+          <t>Médio Pagador</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Sem Risco</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Muito Alto</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>Muito Baixo</t>
+          <t>Sem Risco</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">

</xml_diff>